<commit_message>
Add database and initialize data
</commit_message>
<xml_diff>
--- a/Documents/Data/Dictionaries & Languages/Dictionaries And Language.xlsx
+++ b/Documents/Data/Dictionaries & Languages/Dictionaries And Language.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -197,13 +197,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -211,14 +211,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -543,24 +543,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="90.375" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="18.75" customWidth="1"/>
+    <col min="5" max="5" width="9.625" customWidth="1"/>
     <col min="6" max="6" width="16" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="9" max="9" width="23.25" customWidth="1"/>
+    <col min="10" max="10" width="34.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -656,7 +656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -688,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -720,7 +720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -752,7 +752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -784,7 +784,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -816,7 +816,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -848,7 +848,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -880,7 +880,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>